<commit_message>
Added support for Negro "actually in use" worksheet
</commit_message>
<xml_diff>
--- a/export/debug.xlsx
+++ b/export/debug.xlsx
@@ -68,196 +68,204 @@
     <t>BELVÉDÈRE</t>
   </si>
   <si>
+    <t>BT115
+PARIS DAUPHINE</t>
+  </si>
+  <si>
+    <t>BT131 REPRISE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BT134
+LAYANI </t>
+  </si>
+  <si>
+    <t>BT144 J.D'ARC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BT159 </t>
+  </si>
+  <si>
+    <t>BT160
+UFR 
+ANGERS</t>
+  </si>
+  <si>
+    <t>BT163 TOULOUSE</t>
+  </si>
+  <si>
+    <t>BT171 BESSIER</t>
+  </si>
+  <si>
+    <t>BT172
+TOUR NEPTUNE</t>
+  </si>
+  <si>
+    <t>CARAC</t>
+  </si>
+  <si>
+    <t>CLÉRET</t>
+  </si>
+  <si>
+    <t>CLÉRET 2</t>
+  </si>
+  <si>
+    <t>JEANNE D'ARC</t>
+  </si>
+  <si>
+    <t>LA RAPÉE</t>
+  </si>
+  <si>
+    <t>PD102 LAYANI</t>
+  </si>
+  <si>
+    <t>PD106 TRAPPES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PD117
+CARAC </t>
+  </si>
+  <si>
+    <t>PD13 NANTES</t>
+  </si>
+  <si>
+    <t>PD16
+LA RAPÉE</t>
+  </si>
+  <si>
+    <t>PD18 GUYANCOURT</t>
+  </si>
+  <si>
+    <t>PD36
+R. ALBERT</t>
+  </si>
+  <si>
+    <t>PD38 BESSIER</t>
+  </si>
+  <si>
+    <t>PD39 LIMOURS</t>
+  </si>
+  <si>
+    <t>PD40 BESSIER</t>
+  </si>
+  <si>
+    <t>PD41 BESSIER</t>
+  </si>
+  <si>
+    <t>PD42 BESSIER</t>
+  </si>
+  <si>
+    <t>PD466 COMMYNES</t>
+  </si>
+  <si>
+    <t>PD467 COMMYNES</t>
+  </si>
+  <si>
+    <t>PD58 CLÉRET</t>
+  </si>
+  <si>
+    <t>STEPHENSON</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>X*</t>
+  </si>
+  <si>
+    <t>X**</t>
+  </si>
+  <si>
+    <t>X***</t>
+  </si>
+  <si>
+    <t>X****</t>
+  </si>
+  <si>
+    <t>BT16</t>
+  </si>
+  <si>
+    <t>BT106</t>
+  </si>
+  <si>
+    <t>BT114</t>
+  </si>
+  <si>
     <t>BT115</t>
   </si>
   <si>
+    <t>BT120</t>
+  </si>
+  <si>
+    <t>BT121</t>
+  </si>
+  <si>
+    <t>BT126</t>
+  </si>
+  <si>
     <t>BT131</t>
   </si>
   <si>
     <t>BT134</t>
   </si>
   <si>
+    <t>BT143</t>
+  </si>
+  <si>
     <t>BT144</t>
   </si>
   <si>
+    <t>BT145</t>
+  </si>
+  <si>
+    <t>BT150</t>
+  </si>
+  <si>
+    <t>BT151</t>
+  </si>
+  <si>
+    <t>BT152</t>
+  </si>
+  <si>
+    <t>BT153</t>
+  </si>
+  <si>
+    <t>BT154</t>
+  </si>
+  <si>
+    <t>BT156</t>
+  </si>
+  <si>
+    <t>BT157</t>
+  </si>
+  <si>
+    <t>BT158</t>
+  </si>
+  <si>
     <t>BT159</t>
   </si>
   <si>
     <t>BT160</t>
   </si>
   <si>
+    <t>BT161</t>
+  </si>
+  <si>
     <t>BT163</t>
   </si>
   <si>
+    <t>BT166</t>
+  </si>
+  <si>
+    <t>BT169</t>
+  </si>
+  <si>
+    <t>BT170</t>
+  </si>
+  <si>
     <t>BT171</t>
   </si>
   <si>
     <t>BT172</t>
-  </si>
-  <si>
-    <t>CARAC</t>
-  </si>
-  <si>
-    <t>CLÉRET</t>
-  </si>
-  <si>
-    <t>CLÉRET 2</t>
-  </si>
-  <si>
-    <t>JEANNE D'ARC</t>
-  </si>
-  <si>
-    <t>LA RAPÉE</t>
-  </si>
-  <si>
-    <t>PD102</t>
-  </si>
-  <si>
-    <t>PD106</t>
-  </si>
-  <si>
-    <t>PD117</t>
-  </si>
-  <si>
-    <t>PD13</t>
-  </si>
-  <si>
-    <t>PD16</t>
-  </si>
-  <si>
-    <t>PD18</t>
-  </si>
-  <si>
-    <t>PD36</t>
-  </si>
-  <si>
-    <t>PD38</t>
-  </si>
-  <si>
-    <t>PD39</t>
-  </si>
-  <si>
-    <t>PD40</t>
-  </si>
-  <si>
-    <t>PD41</t>
-  </si>
-  <si>
-    <t>PD42</t>
-  </si>
-  <si>
-    <t>PD466</t>
-  </si>
-  <si>
-    <t>PD467</t>
-  </si>
-  <si>
-    <t>PD58</t>
-  </si>
-  <si>
-    <t>STEPHENSON</t>
-  </si>
-  <si>
-    <t>--</t>
-  </si>
-  <si>
-    <t>---</t>
-  </si>
-  <si>
-    <t>----</t>
-  </si>
-  <si>
-    <t>-----</t>
-  </si>
-  <si>
-    <t>------</t>
-  </si>
-  <si>
-    <t>BT16</t>
-  </si>
-  <si>
-    <t>BT106</t>
-  </si>
-  <si>
-    <t>BT114</t>
-  </si>
-  <si>
-    <t>BT115*</t>
-  </si>
-  <si>
-    <t>BT120</t>
-  </si>
-  <si>
-    <t>BT121</t>
-  </si>
-  <si>
-    <t>BT126</t>
-  </si>
-  <si>
-    <t>BT131*</t>
-  </si>
-  <si>
-    <t>BT134*</t>
-  </si>
-  <si>
-    <t>BT143</t>
-  </si>
-  <si>
-    <t>BT144*</t>
-  </si>
-  <si>
-    <t>BT145</t>
-  </si>
-  <si>
-    <t>BT150</t>
-  </si>
-  <si>
-    <t>BT151</t>
-  </si>
-  <si>
-    <t>BT152</t>
-  </si>
-  <si>
-    <t>BT153</t>
-  </si>
-  <si>
-    <t>BT154</t>
-  </si>
-  <si>
-    <t>BT156</t>
-  </si>
-  <si>
-    <t>BT157</t>
-  </si>
-  <si>
-    <t>BT158</t>
-  </si>
-  <si>
-    <t>BT159*</t>
-  </si>
-  <si>
-    <t>BT160*</t>
-  </si>
-  <si>
-    <t>BT161</t>
-  </si>
-  <si>
-    <t>BT163*</t>
-  </si>
-  <si>
-    <t>BT166</t>
-  </si>
-  <si>
-    <t>BT169</t>
-  </si>
-  <si>
-    <t>BT170</t>
-  </si>
-  <si>
-    <t>BT171*</t>
-  </si>
-  <si>
-    <t>BT172*</t>
   </si>
   <si>
     <t>BT173</t>
@@ -435,52 +443,52 @@
     <col min="17" max="17" width="7.8828125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="7.0625" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="11.25" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="6.6484375" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="6.6484375" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="6.6484375" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="6.6484375" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="6.6484375" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="6.6484375" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="6.6484375" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="6.6484375" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="6.6484375" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="16.296875" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="14.38671875" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="8.05078125" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="13.8828125" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="7.1484375" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="8.39453125" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="16.96484375" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="14.26171875" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="15.27734375" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="7.12109375" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="7.546875" customWidth="true" bestFit="true"/>
     <col min="31" max="31" width="9.16015625" customWidth="true" bestFit="true"/>
     <col min="32" max="32" width="13.9765625" customWidth="true" bestFit="true"/>
     <col min="33" max="33" width="9.484375" customWidth="true" bestFit="true"/>
-    <col min="34" max="34" width="6.87109375" customWidth="true" bestFit="true"/>
-    <col min="35" max="35" width="6.87109375" customWidth="true" bestFit="true"/>
-    <col min="36" max="36" width="6.87109375" customWidth="true" bestFit="true"/>
-    <col min="37" max="37" width="5.75390625" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="5.75390625" customWidth="true" bestFit="true"/>
-    <col min="39" max="39" width="5.75390625" customWidth="true" bestFit="true"/>
-    <col min="40" max="40" width="5.75390625" customWidth="true" bestFit="true"/>
-    <col min="41" max="41" width="5.75390625" customWidth="true" bestFit="true"/>
-    <col min="42" max="42" width="5.75390625" customWidth="true" bestFit="true"/>
-    <col min="43" max="43" width="5.75390625" customWidth="true" bestFit="true"/>
-    <col min="44" max="44" width="5.75390625" customWidth="true" bestFit="true"/>
-    <col min="45" max="45" width="5.75390625" customWidth="true" bestFit="true"/>
-    <col min="46" max="46" width="6.87109375" customWidth="true" bestFit="true"/>
-    <col min="47" max="47" width="6.87109375" customWidth="true" bestFit="true"/>
-    <col min="48" max="48" width="5.75390625" customWidth="true" bestFit="true"/>
+    <col min="34" max="34" width="13.88671875" customWidth="true" bestFit="true"/>
+    <col min="35" max="35" width="15.265625" customWidth="true" bestFit="true"/>
+    <col min="36" max="36" width="7.62109375" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="13.5234375" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="9.484375" customWidth="true" bestFit="true"/>
+    <col min="39" max="39" width="19.125" customWidth="true" bestFit="true"/>
+    <col min="40" max="40" width="10.01953125" customWidth="true" bestFit="true"/>
+    <col min="41" max="41" width="13.3671875" customWidth="true" bestFit="true"/>
+    <col min="42" max="42" width="14.6875" customWidth="true" bestFit="true"/>
+    <col min="43" max="43" width="13.3671875" customWidth="true" bestFit="true"/>
+    <col min="44" max="44" width="13.3671875" customWidth="true" bestFit="true"/>
+    <col min="45" max="45" width="13.3671875" customWidth="true" bestFit="true"/>
+    <col min="46" max="46" width="18.3359375" customWidth="true" bestFit="true"/>
+    <col min="47" max="47" width="18.3359375" customWidth="true" bestFit="true"/>
+    <col min="48" max="48" width="12.765625" customWidth="true" bestFit="true"/>
     <col min="49" max="49" width="13.08203125" customWidth="true" bestFit="true"/>
-    <col min="50" max="50" width="2.3828125" customWidth="true" bestFit="true"/>
-    <col min="51" max="51" width="3.0546875" customWidth="true" bestFit="true"/>
-    <col min="52" max="52" width="3.73046875" customWidth="true" bestFit="true"/>
-    <col min="53" max="53" width="4.40234375" customWidth="true" bestFit="true"/>
-    <col min="54" max="54" width="5.078125" customWidth="true" bestFit="true"/>
+    <col min="50" max="50" width="2.17578125" customWidth="true" bestFit="true"/>
+    <col min="51" max="51" width="3.2734375" customWidth="true" bestFit="true"/>
+    <col min="52" max="52" width="4.3671875" customWidth="true" bestFit="true"/>
+    <col min="53" max="53" width="5.46484375" customWidth="true" bestFit="true"/>
+    <col min="54" max="54" width="6.55859375" customWidth="true" bestFit="true"/>
     <col min="55" max="55" width="5.53515625" customWidth="true" bestFit="true"/>
     <col min="56" max="56" width="6.6484375" customWidth="true" bestFit="true"/>
     <col min="57" max="57" width="6.6484375" customWidth="true" bestFit="true"/>
-    <col min="58" max="58" width="7.74609375" customWidth="true" bestFit="true"/>
+    <col min="58" max="58" width="6.6484375" customWidth="true" bestFit="true"/>
     <col min="59" max="59" width="6.6484375" customWidth="true" bestFit="true"/>
     <col min="60" max="60" width="6.6484375" customWidth="true" bestFit="true"/>
     <col min="61" max="61" width="6.6484375" customWidth="true" bestFit="true"/>
-    <col min="62" max="62" width="7.74609375" customWidth="true" bestFit="true"/>
-    <col min="63" max="63" width="7.74609375" customWidth="true" bestFit="true"/>
+    <col min="62" max="62" width="6.6484375" customWidth="true" bestFit="true"/>
+    <col min="63" max="63" width="6.6484375" customWidth="true" bestFit="true"/>
     <col min="64" max="64" width="6.6484375" customWidth="true" bestFit="true"/>
-    <col min="65" max="65" width="7.74609375" customWidth="true" bestFit="true"/>
+    <col min="65" max="65" width="6.6484375" customWidth="true" bestFit="true"/>
     <col min="66" max="66" width="6.6484375" customWidth="true" bestFit="true"/>
     <col min="67" max="67" width="6.6484375" customWidth="true" bestFit="true"/>
     <col min="68" max="68" width="6.6484375" customWidth="true" bestFit="true"/>
@@ -490,15 +498,15 @@
     <col min="72" max="72" width="6.6484375" customWidth="true" bestFit="true"/>
     <col min="73" max="73" width="6.6484375" customWidth="true" bestFit="true"/>
     <col min="74" max="74" width="6.6484375" customWidth="true" bestFit="true"/>
-    <col min="75" max="75" width="7.74609375" customWidth="true" bestFit="true"/>
-    <col min="76" max="76" width="7.74609375" customWidth="true" bestFit="true"/>
+    <col min="75" max="75" width="6.6484375" customWidth="true" bestFit="true"/>
+    <col min="76" max="76" width="6.6484375" customWidth="true" bestFit="true"/>
     <col min="77" max="77" width="6.6484375" customWidth="true" bestFit="true"/>
-    <col min="78" max="78" width="7.74609375" customWidth="true" bestFit="true"/>
+    <col min="78" max="78" width="6.6484375" customWidth="true" bestFit="true"/>
     <col min="79" max="79" width="6.6484375" customWidth="true" bestFit="true"/>
     <col min="80" max="80" width="6.6484375" customWidth="true" bestFit="true"/>
     <col min="81" max="81" width="6.6484375" customWidth="true" bestFit="true"/>
-    <col min="82" max="82" width="7.74609375" customWidth="true" bestFit="true"/>
-    <col min="83" max="83" width="7.74609375" customWidth="true" bestFit="true"/>
+    <col min="82" max="82" width="6.6484375" customWidth="true" bestFit="true"/>
+    <col min="83" max="83" width="6.6484375" customWidth="true" bestFit="true"/>
     <col min="84" max="84" width="6.6484375" customWidth="true" bestFit="true"/>
     <col min="85" max="85" width="6.6484375" customWidth="true" bestFit="true"/>
     <col min="86" max="86" width="6.6484375" customWidth="true" bestFit="true"/>
@@ -1013,11 +1021,21 @@
       <c r="AW4" t="n">
         <v>0.0</v>
       </c>
-      <c r="AX4"/>
-      <c r="AY4"/>
-      <c r="AZ4"/>
-      <c r="BA4"/>
-      <c r="BB4"/>
+      <c r="AX4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AY4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AZ4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BA4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BB4" t="n">
+        <v>0.0</v>
+      </c>
       <c r="BC4" t="n">
         <v>0.0</v>
       </c>

</xml_diff>